<commit_message>
doc: add new logboek
</commit_message>
<xml_diff>
--- a/docs/DTT logboek.xlsx
+++ b/docs/DTT logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Th3-C\Desktop\projects\dtt\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C47F5195-5DA1-410E-B948-0E7A7AFB1E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F5D595-EE6D-42B6-9882-A82573DB2100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <r>
       <rPr>
@@ -190,13 +190,36 @@
   <si>
     <t>Make this extra entry point to provide the room types the API provide</t>
   </si>
+  <si>
+    <t>Fix login</t>
+  </si>
+  <si>
+    <t>I have forgotten to add some env. Variables to the example</t>
+  </si>
+  <si>
+    <t>Refactor services make them repositories</t>
+  </si>
+  <si>
+    <t>I move the services to the repositories then separate the request logic and moved it to the controllers</t>
+  </si>
+  <si>
+    <t>Make better function doc</t>
+  </si>
+  <si>
+    <t>In the same time I work on the refactoring I change/add comments doc</t>
+  </si>
+  <si>
+    <t>Improve ACL workflow</t>
+  </si>
+  <si>
+    <t>I moved the validation of the JWT token to the ACL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
@@ -489,7 +512,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -500,9 +523,6 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -514,16 +534,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,6 +542,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -544,12 +558,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1810,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -1825,406 +1833,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="11"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="60" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="61.5" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="17">
         <v>4</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="16">
         <v>44171</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="17">
         <v>4</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="16">
         <v>44171</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="44.25" customHeight="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="17">
         <v>6</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="16">
         <v>44172</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="17">
         <v>0.5</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="16">
         <v>44173</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="21.75" customHeight="1">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="17">
         <v>3</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="16">
         <v>44173</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="18" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="81.75" customHeight="1">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="17">
         <v>6</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="16">
         <v>44175</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="18" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="16">
         <v>44176</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="45" customHeight="1">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="17">
         <v>4</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="16">
         <v>44176</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="18" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="47.25" customHeight="1">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="16">
         <v>44177</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="17">
         <v>0.5</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="16">
         <v>44177</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="18" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="24" customHeight="1">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="17">
         <v>1.5</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="16">
         <v>44177</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="17">
         <v>4</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="16">
         <v>44177</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="17">
         <v>4</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="16">
         <v>44178</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="17">
         <v>1</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="16">
         <v>44178</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="18" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="17">
         <v>2</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="16">
         <v>44178</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="18" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="17">
         <v>2</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="16">
         <v>44178</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="18" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="17">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="16">
         <v>44179</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>3</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="16">
         <v>44179</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="18" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="24" customHeight="1">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>3</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="16">
         <v>44179</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="18" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="28"/>
+      <c r="A23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="C23" s="16">
+        <v>44188</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="6"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="28"/>
+    <row r="24" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="17">
+        <v>4</v>
+      </c>
+      <c r="C24" s="16">
+        <v>44188</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="28"/>
+      <c r="A25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="17">
+        <v>1</v>
+      </c>
+      <c r="C25" s="16">
+        <v>44188</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="16"/>
+      <c r="A26" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="16">
+        <v>44188</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="16"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="3"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="6"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="16"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="3"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <f>SUM(B4:B28)</f>
-        <v>53.5</v>
+        <v>59.25</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2232,7 +2272,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A31" s="7"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2240,7 +2280,7 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2248,12 +2288,12 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>